<commit_message>
linear regression and meta analysis for speed
</commit_message>
<xml_diff>
--- a/Results/NEW_periods/Baseline/Female/meta_analysis_treatment_vs_control.xlsx
+++ b/Results/NEW_periods/Baseline/Female/meta_analysis_treatment_vs_control.xlsx
@@ -352,7 +352,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -394,13 +394,13 @@
         </is>
       </c>
       <c r="B3">
-        <v>0.5959456762033492</v>
+        <v>0.5959455751686174</v>
       </c>
       <c r="C3">
-        <v>1.013994037714918</v>
+        <v>1.013994367340575</v>
       </c>
       <c r="D3">
-        <v>1.61569319096323</v>
+        <v>1.615694245733231</v>
       </c>
     </row>
     <row r="4">
@@ -410,13 +410,13 @@
         </is>
       </c>
       <c r="B4">
-        <v>0.4618511457083053</v>
+        <v>0.4618510332094891</v>
       </c>
       <c r="C4">
-        <v>1.287830652095633</v>
+        <v>1.287831479938114</v>
       </c>
       <c r="D4">
-        <v>2.529850437886088</v>
+        <v>2.529853038381398</v>
       </c>
     </row>
     <row r="5">
@@ -426,13 +426,13 @@
         </is>
       </c>
       <c r="B5">
-        <v>0.6941223002978367</v>
+        <v>0.6941222355568236</v>
       </c>
       <c r="C5">
-        <v>1.159082539215658</v>
+        <v>1.159082944814026</v>
       </c>
       <c r="D5">
-        <v>1.624547477481751</v>
+        <v>1.6245483587712</v>
       </c>
     </row>
     <row r="6">
@@ -449,13 +449,13 @@
         </is>
       </c>
       <c r="B7">
-        <v>26.325218170253</v>
+        <v>26.32521348497664</v>
       </c>
       <c r="C7">
-        <v>35.81364741152617</v>
+        <v>35.813664395729</v>
       </c>
       <c r="D7">
-        <v>47.62545071731759</v>
+        <v>47.62549860435363</v>
       </c>
     </row>
     <row r="8">
@@ -465,13 +465,13 @@
         </is>
       </c>
       <c r="B8">
-        <v>0.1999869848385824</v>
+        <v>0.1999870001396751</v>
       </c>
       <c r="C8">
-        <v>0.4613819816984409</v>
+        <v>0.461383181708975</v>
       </c>
       <c r="D8">
-        <v>0.8301616298945221</v>
+        <v>0.8301648248825331</v>
       </c>
     </row>
     <row r="9">
@@ -481,13 +481,13 @@
         </is>
       </c>
       <c r="B9">
-        <v>0.4540789199065468</v>
+        <v>0.4540789713723684</v>
       </c>
       <c r="C9">
-        <v>0.6897008948054523</v>
+        <v>0.6897018435148856</v>
       </c>
       <c r="D9">
-        <v>0.9251492532289946</v>
+        <v>0.9251511029733821</v>
       </c>
     </row>
     <row r="10">
@@ -504,13 +504,13 @@
         </is>
       </c>
       <c r="B11">
-        <v>6.123347621576404</v>
+        <v>6.123347660593229</v>
       </c>
       <c r="C11">
-        <v>8.77599708967491</v>
+        <v>8.775997425171873</v>
       </c>
       <c r="D11">
-        <v>12.17825156070624</v>
+        <v>12.17825231403138</v>
       </c>
     </row>
     <row r="12">
@@ -520,13 +520,13 @@
         </is>
       </c>
       <c r="B12">
-        <v>0.235330610222909</v>
+        <v>0.2353306090000331</v>
       </c>
       <c r="C12">
-        <v>0.5852165189723945</v>
+        <v>0.5852165482337847</v>
       </c>
       <c r="D12">
-        <v>1.091708781119589</v>
+        <v>1.091708863976712</v>
       </c>
     </row>
     <row r="13">
@@ -536,13 +536,68 @@
         </is>
       </c>
       <c r="B13">
-        <v>0.4936927336274102</v>
+        <v>0.4936927331846208</v>
       </c>
       <c r="C13">
-        <v>0.7785308255377978</v>
+        <v>0.7785308463259701</v>
       </c>
       <c r="D13">
-        <v>1.063337001317083</v>
+        <v>1.063337043478054</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Speed meta analysis</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>mean (km/day)</t>
+        </is>
+      </c>
+      <c r="B15">
+        <v>4.112431376685026</v>
+      </c>
+      <c r="C15">
+        <v>4.760985039628134</v>
+      </c>
+      <c r="D15">
+        <v>5.480449112430368</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>CoV² (RVAR)</t>
+        </is>
+      </c>
+      <c r="B16">
+        <v>0.03542117434183563</v>
+      </c>
+      <c r="C16">
+        <v>0.0851651924223696</v>
+      </c>
+      <c r="D16">
+        <v>0.1563522747651325</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>CoV  (RSTD)</t>
+        </is>
+      </c>
+      <c r="B17">
+        <v>0.191337966285609</v>
+      </c>
+      <c r="C17">
+        <v>0.2966885197628259</v>
+      </c>
+      <c r="D17">
+        <v>0.4019960427239915</v>
       </c>
     </row>
   </sheetData>
@@ -552,7 +607,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -594,13 +649,13 @@
         </is>
       </c>
       <c r="B3">
-        <v>41.08416648947812</v>
+        <v>41.0841764212609</v>
       </c>
       <c r="C3">
-        <v>52.24317107289249</v>
+        <v>52.24317489057803</v>
       </c>
       <c r="D3">
-        <v>65.47939256936198</v>
+        <v>65.47938736384387</v>
       </c>
     </row>
     <row r="4">
@@ -610,13 +665,13 @@
         </is>
       </c>
       <c r="B4">
-        <v>0.07954458769690034</v>
+        <v>0.07954459666577422</v>
       </c>
       <c r="C4">
-        <v>0.207384045126219</v>
+        <v>0.2073836971666101</v>
       </c>
       <c r="D4">
-        <v>0.3954049823020335</v>
+        <v>0.3954039972050888</v>
       </c>
     </row>
     <row r="5">
@@ -626,13 +681,13 @@
         </is>
       </c>
       <c r="B5">
-        <v>0.287449639276553</v>
+        <v>0.2874496393090814</v>
       </c>
       <c r="C5">
-        <v>0.4641347880712924</v>
+        <v>0.4641343725828301</v>
       </c>
       <c r="D5">
-        <v>0.6408811810951705</v>
+        <v>0.640880346703167</v>
       </c>
     </row>
     <row r="6">
@@ -649,13 +704,13 @@
         </is>
       </c>
       <c r="B7">
-        <v>19.10688363496106</v>
+        <v>19.1068835724091</v>
       </c>
       <c r="C7">
-        <v>22.32140991191142</v>
+        <v>22.32140647266363</v>
       </c>
       <c r="D7">
-        <v>25.91730957643812</v>
+        <v>25.91730203741737</v>
       </c>
     </row>
     <row r="8">
@@ -665,13 +720,13 @@
         </is>
       </c>
       <c r="B8">
-        <v>0.03582192168406915</v>
+        <v>0.03582192564724802</v>
       </c>
       <c r="C8">
-        <v>0.08946566044612725</v>
+        <v>0.08946553009626575</v>
       </c>
       <c r="D8">
-        <v>0.1672331244462449</v>
+        <v>0.1672327581618985</v>
       </c>
     </row>
     <row r="9">
@@ -681,13 +736,13 @@
         </is>
       </c>
       <c r="B9">
-        <v>0.1926414043170306</v>
+        <v>0.192641405648309</v>
       </c>
       <c r="C9">
-        <v>0.3044411695137165</v>
+        <v>0.3044409329938641</v>
       </c>
       <c r="D9">
-        <v>0.4162328449217795</v>
+        <v>0.4162323689434379</v>
       </c>
     </row>
     <row r="10">
@@ -704,13 +759,13 @@
         </is>
       </c>
       <c r="B11">
-        <v>5.318410701891304</v>
+        <v>5.318410720789306</v>
       </c>
       <c r="C11">
-        <v>6.523880221784932</v>
+        <v>6.523880458632495</v>
       </c>
       <c r="D11">
-        <v>7.916469290196163</v>
+        <v>7.916469803675057</v>
       </c>
     </row>
     <row r="12">
@@ -720,13 +775,13 @@
         </is>
       </c>
       <c r="B12">
-        <v>0.05417348386788978</v>
+        <v>0.054173483368058</v>
       </c>
       <c r="C12">
-        <v>0.14634655939998</v>
+        <v>0.1463465908338701</v>
       </c>
       <c r="D12">
-        <v>0.2835157108716778</v>
+        <v>0.2835157999455275</v>
       </c>
     </row>
     <row r="13">
@@ -736,13 +791,68 @@
         </is>
       </c>
       <c r="B13">
-        <v>0.2374859497431381</v>
+        <v>0.2374859503411489</v>
       </c>
       <c r="C13">
-        <v>0.3903334734432736</v>
+        <v>0.3903335181468861</v>
       </c>
       <c r="D13">
-        <v>0.5432917409101755</v>
+        <v>0.5432918301291978</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Speed meta analysis</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>mean (km/day)</t>
+        </is>
+      </c>
+      <c r="B15">
+        <v>3.633749656974639</v>
+      </c>
+      <c r="C15">
+        <v>4.280444381018343</v>
+      </c>
+      <c r="D15">
+        <v>5.005375851837153</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>CoV² (RVAR)</t>
+        </is>
+      </c>
+      <c r="B16">
+        <v>0.02156303552970272</v>
+      </c>
+      <c r="C16">
+        <v>0.07173901326442587</v>
+      </c>
+      <c r="D16">
+        <v>0.151526132229185</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>CoV  (RSTD)</t>
+        </is>
+      </c>
+      <c r="B17">
+        <v>0.1508584116135067</v>
+      </c>
+      <c r="C17">
+        <v>0.2751644225042091</v>
+      </c>
+      <c r="D17">
+        <v>0.3999063961861548</v>
       </c>
     </row>
   </sheetData>

</xml_diff>